<commit_message>
Renamed: the main class to BpmfSyllable to avoid confusion; Added: hashCode, op= and comparable implementation
</commit_message>
<xml_diff>
--- a/data/py_data.xlsx
+++ b/data/py_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proj\linguistics\hiunnsjv\bpmf_py\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125CD6DD-5F6A-41D5-B08B-3077530C28D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE924EDF-6651-4FDC-81D0-5D12447CD7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2C83AE64-0DDA-41B2-B186-7088351FE75B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{2C83AE64-0DDA-41B2-B186-7088351FE75B}"/>
   </bookViews>
   <sheets>
     <sheet name="all_sounds" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3323" uniqueCount="2922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3321" uniqueCount="2921">
   <si>
     <t>ㄅㄚ</t>
   </si>
@@ -8794,10 +8794,6 @@
   </si>
   <si>
     <t>e</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>ê</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -35390,10 +35386,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A7BA11-B902-4F19-9D4B-67E2E5462451}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -35417,7 +35413,7 @@
         <v>2824</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -35458,7 +35454,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>2838</v>
+        <v>2825</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>2882</v>
@@ -35469,7 +35465,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>2825</v>
+        <v>2841</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>2883</v>
@@ -35480,7 +35476,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>2841</v>
+        <v>2830</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>2884</v>
@@ -35491,7 +35487,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>2830</v>
+        <v>2855</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>2885</v>
@@ -35502,7 +35498,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>2855</v>
+        <v>2827</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>2886</v>
@@ -35513,7 +35509,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>2827</v>
+        <v>2842</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>2887</v>
@@ -35524,20 +35520,20 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>2842</v>
+        <v>2828</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>2888</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>2828</v>
-      </c>
-      <c r="C13" s="6" t="s">
+        <v>2844</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>2889</v>
       </c>
     </row>
@@ -35546,20 +35542,20 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>2844</v>
-      </c>
-      <c r="C14" s="7" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>2890</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2846</v>
+      </c>
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>2891</v>
       </c>
     </row>
@@ -35567,10 +35563,10 @@
       <c r="A16" t="s">
         <v>2846</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" t="s">
+        <v>2824</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>2892</v>
       </c>
     </row>
@@ -35579,7 +35575,7 @@
         <v>2846</v>
       </c>
       <c r="B17" t="s">
-        <v>2824</v>
+        <v>2856</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>2893</v>
@@ -35590,7 +35586,7 @@
         <v>2846</v>
       </c>
       <c r="B18" t="s">
-        <v>2856</v>
+        <v>2839</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>2894</v>
@@ -35601,7 +35597,7 @@
         <v>2846</v>
       </c>
       <c r="B19" t="s">
-        <v>2839</v>
+        <v>2825</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>2895</v>
@@ -35612,7 +35608,7 @@
         <v>2846</v>
       </c>
       <c r="B20" t="s">
-        <v>2825</v>
+        <v>2830</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>2896</v>
@@ -35623,7 +35619,7 @@
         <v>2846</v>
       </c>
       <c r="B21" t="s">
-        <v>2830</v>
+        <v>2855</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>2897</v>
@@ -35634,7 +35630,7 @@
         <v>2846</v>
       </c>
       <c r="B22" t="s">
-        <v>2855</v>
+        <v>2827</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>2898</v>
@@ -35645,7 +35641,7 @@
         <v>2846</v>
       </c>
       <c r="B23" t="s">
-        <v>2827</v>
+        <v>2842</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>2899</v>
@@ -35656,31 +35652,31 @@
         <v>2846</v>
       </c>
       <c r="B24" t="s">
-        <v>2842</v>
+        <v>2828</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>2900</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2846</v>
       </c>
       <c r="B25" t="s">
-        <v>2828</v>
-      </c>
-      <c r="C25" s="6" t="s">
+        <v>2844</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>2901</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2846</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2844</v>
-      </c>
-      <c r="C26" s="7" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>2902</v>
       </c>
     </row>
@@ -35688,10 +35684,10 @@
       <c r="A27" t="s">
         <v>2859</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B27" t="s">
+        <v>2824</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>2903</v>
       </c>
     </row>
@@ -35700,10 +35696,10 @@
         <v>2859</v>
       </c>
       <c r="B28" t="s">
-        <v>2824</v>
+        <v>2838</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>2904</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -35711,10 +35707,10 @@
         <v>2859</v>
       </c>
       <c r="B29" t="s">
-        <v>2838</v>
+        <v>2856</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>2865</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -35722,7 +35718,7 @@
         <v>2859</v>
       </c>
       <c r="B30" t="s">
-        <v>2856</v>
+        <v>2825</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>2905</v>
@@ -35733,7 +35729,7 @@
         <v>2859</v>
       </c>
       <c r="B31" t="s">
-        <v>2825</v>
+        <v>2841</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>2906</v>
@@ -35744,7 +35740,7 @@
         <v>2859</v>
       </c>
       <c r="B32" t="s">
-        <v>2841</v>
+        <v>2827</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>2907</v>
@@ -35755,7 +35751,7 @@
         <v>2859</v>
       </c>
       <c r="B33" t="s">
-        <v>2827</v>
+        <v>2842</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>2908</v>
@@ -35766,31 +35762,31 @@
         <v>2859</v>
       </c>
       <c r="B34" t="s">
-        <v>2842</v>
+        <v>2828</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>2909</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2859</v>
       </c>
       <c r="B35" t="s">
-        <v>2828</v>
-      </c>
-      <c r="C35" s="6" t="s">
+        <v>2844</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>2910</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>2859</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2844</v>
-      </c>
-      <c r="C36" s="7" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>2911</v>
       </c>
     </row>
@@ -35798,10 +35794,10 @@
       <c r="A37" t="s">
         <v>2862</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B37" t="s">
+        <v>2838</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>2912</v>
       </c>
     </row>
@@ -35810,7 +35806,7 @@
         <v>2862</v>
       </c>
       <c r="B38" t="s">
-        <v>2838</v>
+        <v>2827</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>2913</v>
@@ -35821,31 +35817,31 @@
         <v>2862</v>
       </c>
       <c r="B39" t="s">
-        <v>2827</v>
+        <v>2842</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>2914</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2862</v>
       </c>
       <c r="B40" t="s">
-        <v>2842</v>
-      </c>
-      <c r="C40" s="6" t="s">
+        <v>2844</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>2915</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>2862</v>
       </c>
-      <c r="B41" t="s">
-        <v>2844</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>2916</v>
       </c>
     </row>
@@ -35853,8 +35849,8 @@
       <c r="A42" t="s">
         <v>2862</v>
       </c>
-      <c r="B42">
-        <v>0</v>
+      <c r="B42" t="s">
+        <v>2838</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>2917</v>
@@ -35865,7 +35861,7 @@
         <v>2862</v>
       </c>
       <c r="B43" t="s">
-        <v>2838</v>
+        <v>2827</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>2918</v>
@@ -35876,21 +35872,10 @@
         <v>2862</v>
       </c>
       <c r="B44" t="s">
-        <v>2827</v>
+        <v>2842</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>2919</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>2862</v>
-      </c>
-      <c r="B45" t="s">
-        <v>2842</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>2920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>